<commit_message>
Adding flash alerts and express sessions
</commit_message>
<xml_diff>
--- a/donetill.xlsx
+++ b/donetill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DELTA\Wanderlust\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAC44D2-9365-4749-BB14-F151A97101FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760D1BF7-BE51-42F1-BB75-B9C17BD2E8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3588" yWindow="2424" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,7 +482,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added user model and authentication
</commit_message>
<xml_diff>
--- a/donetill.xlsx
+++ b/donetill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DELTA\Wanderlust\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760D1BF7-BE51-42F1-BB75-B9C17BD2E8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96513ED4-6254-44BD-9B7B-01A9BAE74228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3588" yWindow="2424" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,7 +487,7 @@
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor passport functions added
</commit_message>
<xml_diff>
--- a/donetill.xlsx
+++ b/donetill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DELTA\Wanderlust\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96513ED4-6254-44BD-9B7B-01A9BAE74228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D6BA70-DC33-40FB-B6F4-2DD29A4BF6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3588" yWindow="2424" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Create basic DB</t>
   </si>
@@ -72,13 +72,16 @@
     <t>database relationships</t>
   </si>
   <si>
-    <t>password hashing</t>
-  </si>
-  <si>
     <t>handling deletions(cascading deletions)</t>
   </si>
   <si>
     <t>review model</t>
+  </si>
+  <si>
+    <t>authentication</t>
+  </si>
+  <si>
+    <t>authorization</t>
   </si>
 </sst>
 </file>
@@ -120,9 +123,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,12 +477,12 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -492,8 +496,13 @@
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>15</v>
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>